<commit_message>
Improve xloIndex to handle missing arguments more naturally and more like the INDEX function in Office 365.  Add a sneaky array view option into xloper12, so xloIndex can return some array slices without copying
tests: add tests for new syntax
</commit_message>
<xml_diff>
--- a/tests/AutoSheets/TestUtils.xlsx
+++ b/tests/AutoSheets/TestUtils.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\tests\AutoSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil_build\tests\AutoSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BA0DE9-9491-4F30-88FB-FBE6A1AA50DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA19D365-8563-467A-98E1-623EEEEDA4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Block-Fill-FillNA" sheetId="1" r:id="rId1"/>
@@ -57,6 +57,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -86,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="94">
   <si>
     <t>1, 2; 3, 4;</t>
   </si>
@@ -362,6 +363,12 @@
   </si>
   <si>
     <t>another|domain</t>
+  </si>
+  <si>
+    <t>xloIndex: single row</t>
+  </si>
+  <si>
+    <t>xloIndex: single column</t>
   </si>
 </sst>
 </file>
@@ -2188,7 +2195,7 @@
       </c>
       <c r="S8" s="7">
         <f ca="1">RAND()</f>
-        <v>0.78896272738121298</v>
+        <v>0.70907073699696899</v>
       </c>
       <c r="T8" s="4">
         <f t="array" aca="1" ref="T8:T107" ca="1">_xll.xloSort(S8:S107,"a")</f>
@@ -3510,7 +3517,7 @@
       </c>
       <c r="T77" s="4">
         <f ca="1"/>
-        <v>0.71755405184921206</v>
+        <v>0.70907073699696899</v>
       </c>
     </row>
     <row r="78" spans="19:20">
@@ -3519,7 +3526,7 @@
       </c>
       <c r="T78" s="4">
         <f ca="1"/>
-        <v>0.73492497530386436</v>
+        <v>0.71755405184921206</v>
       </c>
     </row>
     <row r="79" spans="19:20">
@@ -3528,7 +3535,7 @@
       </c>
       <c r="T79" s="4">
         <f ca="1"/>
-        <v>0.78402600397426425</v>
+        <v>0.73492497530386436</v>
       </c>
     </row>
     <row r="80" spans="19:20">
@@ -3537,7 +3544,7 @@
       </c>
       <c r="T80" s="4">
         <f ca="1"/>
-        <v>0.78896272738121298</v>
+        <v>0.78402600397426425</v>
       </c>
     </row>
     <row r="81" spans="19:20">
@@ -3796,10 +3803,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="B2:M18"/>
+  <dimension ref="B2:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4011,6 +4018,63 @@
         <v>9</v>
       </c>
     </row>
+    <row r="20" spans="2:7">
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="10" t="b" cm="1">
+        <f t="array" ref="C20">SUM(0+(_xlfn.ANCHORARRAY(D20)=F3:H3))=3</f>
+        <v>1</v>
+      </c>
+      <c r="D20" cm="1">
+        <f t="array" ref="D20:F20">_xll.xloIndex($E$3,1)</f>
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="10" t="b" cm="1">
+        <f t="array" ref="C22">SUM(0+(_xlfn.ANCHORARRAY(D22)=H3:H5))=3</f>
+        <v>1</v>
+      </c>
+      <c r="D22" cm="1">
+        <f t="array" ref="D22:F22">TRANSPOSE(_xll.xloIndex($E$3,,-1))</f>
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>6</v>
+      </c>
+      <c r="F22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="C25" s="10" t="b" cm="1">
+        <f t="array" ref="C25">SUM(0+(D25:E25=F25:G25))=2</f>
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
+      <c r="F25" s="5" cm="1">
+        <f t="array" ref="F25:G25">_xll.xloIndex(K3:M5,2,2,,0)</f>
+        <v>5</v>
+      </c>
+      <c r="G25" s="5">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4021,8 +4085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09126F57-EC62-4488-961C-3C6B3640DBE9}">
   <dimension ref="B2:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Merge 0.17.11 to master
</commit_message>
<xml_diff>
--- a/tests/AutoSheets/TestUtils.xlsx
+++ b/tests/AutoSheets/TestUtils.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil\tests\AutoSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steven\dev\xloil_build\tests\AutoSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BA0DE9-9491-4F30-88FB-FBE6A1AA50DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA19D365-8563-467A-98E1-623EEEEDA4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Block-Fill-FillNA" sheetId="1" r:id="rId1"/>
@@ -57,6 +57,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -86,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="94">
   <si>
     <t>1, 2; 3, 4;</t>
   </si>
@@ -362,6 +363,12 @@
   </si>
   <si>
     <t>another|domain</t>
+  </si>
+  <si>
+    <t>xloIndex: single row</t>
+  </si>
+  <si>
+    <t>xloIndex: single column</t>
   </si>
 </sst>
 </file>
@@ -2188,7 +2195,7 @@
       </c>
       <c r="S8" s="7">
         <f ca="1">RAND()</f>
-        <v>0.78896272738121298</v>
+        <v>0.70907073699696899</v>
       </c>
       <c r="T8" s="4">
         <f t="array" aca="1" ref="T8:T107" ca="1">_xll.xloSort(S8:S107,"a")</f>
@@ -3510,7 +3517,7 @@
       </c>
       <c r="T77" s="4">
         <f ca="1"/>
-        <v>0.71755405184921206</v>
+        <v>0.70907073699696899</v>
       </c>
     </row>
     <row r="78" spans="19:20">
@@ -3519,7 +3526,7 @@
       </c>
       <c r="T78" s="4">
         <f ca="1"/>
-        <v>0.73492497530386436</v>
+        <v>0.71755405184921206</v>
       </c>
     </row>
     <row r="79" spans="19:20">
@@ -3528,7 +3535,7 @@
       </c>
       <c r="T79" s="4">
         <f ca="1"/>
-        <v>0.78402600397426425</v>
+        <v>0.73492497530386436</v>
       </c>
     </row>
     <row r="80" spans="19:20">
@@ -3537,7 +3544,7 @@
       </c>
       <c r="T80" s="4">
         <f ca="1"/>
-        <v>0.78896272738121298</v>
+        <v>0.78402600397426425</v>
       </c>
     </row>
     <row r="81" spans="19:20">
@@ -3796,10 +3803,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="B2:M18"/>
+  <dimension ref="B2:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4011,6 +4018,63 @@
         <v>9</v>
       </c>
     </row>
+    <row r="20" spans="2:7">
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="10" t="b" cm="1">
+        <f t="array" ref="C20">SUM(0+(_xlfn.ANCHORARRAY(D20)=F3:H3))=3</f>
+        <v>1</v>
+      </c>
+      <c r="D20" cm="1">
+        <f t="array" ref="D20:F20">_xll.xloIndex($E$3,1)</f>
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="10" t="b" cm="1">
+        <f t="array" ref="C22">SUM(0+(_xlfn.ANCHORARRAY(D22)=H3:H5))=3</f>
+        <v>1</v>
+      </c>
+      <c r="D22" cm="1">
+        <f t="array" ref="D22:F22">TRANSPOSE(_xll.xloIndex($E$3,,-1))</f>
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>6</v>
+      </c>
+      <c r="F22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="C25" s="10" t="b" cm="1">
+        <f t="array" ref="C25">SUM(0+(D25:E25=F25:G25))=2</f>
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
+      <c r="F25" s="5" cm="1">
+        <f t="array" ref="F25:G25">_xll.xloIndex(K3:M5,2,2,,0)</f>
+        <v>5</v>
+      </c>
+      <c r="G25" s="5">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4021,8 +4085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09126F57-EC62-4488-961C-3C6B3640DBE9}">
   <dimension ref="B2:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>